<commit_message>
Adjusted the F4 model accroding to v1.1 of instruction packet - 1 voltage bus / 6xCB
</commit_message>
<xml_diff>
--- a/DistributionSystems/SimulinkOpal/Banshee/relay_settings/F4_relay_nrel.xlsx
+++ b/DistributionSystems/SimulinkOpal/Banshee/relay_settings/F4_relay_nrel.xlsx
@@ -68,7 +68,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -87,13 +87,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -150,7 +143,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -185,9 +178,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -218,7 +208,7 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="6225872" cy="4914679"/>
@@ -782,10 +772,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V19"/>
+  <dimension ref="A1:V12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -897,7 +887,7 @@
       <c r="F2" s="5">
         <v>2</v>
       </c>
-      <c r="G2" s="13">
+      <c r="G2" s="12">
         <v>3500</v>
       </c>
       <c r="H2" s="11">
@@ -909,7 +899,7 @@
       <c r="J2" s="6">
         <v>0</v>
       </c>
-      <c r="K2" s="14">
+      <c r="K2" s="13">
         <v>0.80187537387448016</v>
       </c>
       <c r="L2" s="6">
@@ -930,7 +920,7 @@
       <c r="Q2" s="6">
         <v>0</v>
       </c>
-      <c r="R2" s="14">
+      <c r="R2" s="13">
         <v>0.80187537387448016</v>
       </c>
       <c r="S2" s="6">
@@ -965,7 +955,7 @@
       <c r="F3" s="5">
         <v>2</v>
       </c>
-      <c r="G3" s="13">
+      <c r="G3" s="12">
         <v>3500</v>
       </c>
       <c r="H3" s="11">
@@ -977,7 +967,7 @@
       <c r="J3" s="6">
         <v>0</v>
       </c>
-      <c r="K3" s="14">
+      <c r="K3" s="13">
         <v>0.20046884346862004</v>
       </c>
       <c r="L3" s="6">
@@ -998,7 +988,7 @@
       <c r="Q3" s="6">
         <v>0</v>
       </c>
-      <c r="R3" s="14">
+      <c r="R3" s="13">
         <v>0.20046884346862004</v>
       </c>
       <c r="S3" s="6">
@@ -1033,7 +1023,7 @@
       <c r="F4" s="5">
         <v>2</v>
       </c>
-      <c r="G4" s="13">
+      <c r="G4" s="12">
         <v>3500</v>
       </c>
       <c r="H4" s="11">
@@ -1045,7 +1035,7 @@
       <c r="J4" s="6">
         <v>0</v>
       </c>
-      <c r="K4" s="14">
+      <c r="K4" s="13">
         <v>0.90210979560879001</v>
       </c>
       <c r="L4" s="6">
@@ -1066,7 +1056,7 @@
       <c r="Q4" s="6">
         <v>0</v>
       </c>
-      <c r="R4" s="14">
+      <c r="R4" s="13">
         <v>0.90210979560879001</v>
       </c>
       <c r="S4" s="6">
@@ -1101,7 +1091,7 @@
       <c r="F5" s="5">
         <v>2</v>
       </c>
-      <c r="G5" s="13">
+      <c r="G5" s="12">
         <v>3500</v>
       </c>
       <c r="H5" s="11">
@@ -1113,7 +1103,7 @@
       <c r="J5" s="6">
         <v>0</v>
       </c>
-      <c r="K5" s="14">
+      <c r="K5" s="13">
         <v>0.50117210867155004</v>
       </c>
       <c r="L5" s="6">
@@ -1134,7 +1124,7 @@
       <c r="Q5" s="6">
         <v>0</v>
       </c>
-      <c r="R5" s="14">
+      <c r="R5" s="13">
         <v>0.50117210867155004</v>
       </c>
       <c r="S5" s="6">
@@ -1169,7 +1159,7 @@
       <c r="F6" s="5">
         <v>2</v>
       </c>
-      <c r="G6" s="13">
+      <c r="G6" s="12">
         <v>3500</v>
       </c>
       <c r="H6" s="11">
@@ -1181,7 +1171,7 @@
       <c r="J6" s="6">
         <v>0</v>
       </c>
-      <c r="K6" s="14">
+      <c r="K6" s="13">
         <v>0.40093768693724008</v>
       </c>
       <c r="L6" s="6">
@@ -1202,7 +1192,7 @@
       <c r="Q6" s="6">
         <v>0</v>
       </c>
-      <c r="R6" s="14">
+      <c r="R6" s="13">
         <v>0.40093768693724008</v>
       </c>
       <c r="S6" s="6">
@@ -1237,7 +1227,7 @@
       <c r="F7" s="5">
         <v>2</v>
       </c>
-      <c r="G7" s="13">
+      <c r="G7" s="12">
         <v>3500</v>
       </c>
       <c r="H7" s="11">
@@ -1249,7 +1239,7 @@
       <c r="J7" s="6">
         <v>0</v>
       </c>
-      <c r="K7" s="14">
+      <c r="K7" s="13">
         <v>0.40093768693724008</v>
       </c>
       <c r="L7" s="6">
@@ -1270,7 +1260,7 @@
       <c r="Q7" s="6">
         <v>0</v>
       </c>
-      <c r="R7" s="14">
+      <c r="R7" s="13">
         <v>0.40093768693724008</v>
       </c>
       <c r="S7" s="6">
@@ -1287,535 +1277,59 @@
       </c>
     </row>
     <row r="8" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A8" s="8">
-        <v>7</v>
-      </c>
-      <c r="B8" s="6">
-        <v>480</v>
-      </c>
-      <c r="C8" s="5">
-        <v>10</v>
-      </c>
-      <c r="D8" s="5">
-        <v>12</v>
-      </c>
-      <c r="E8" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="F8" s="5">
-        <v>2</v>
-      </c>
-      <c r="G8" s="13">
-        <v>3500</v>
-      </c>
-      <c r="H8" s="11">
-        <v>0</v>
-      </c>
-      <c r="I8" s="6">
-        <v>20</v>
-      </c>
-      <c r="J8" s="6">
-        <v>0</v>
-      </c>
-      <c r="K8" s="14">
-        <v>1.1856300170858387</v>
-      </c>
-      <c r="L8" s="6">
-        <v>1</v>
-      </c>
-      <c r="M8" s="6">
-        <v>1</v>
-      </c>
-      <c r="N8" s="6">
-        <v>0.7</v>
-      </c>
-      <c r="O8" s="6">
-        <v>1.2</v>
-      </c>
-      <c r="P8" s="6">
-        <v>20</v>
-      </c>
-      <c r="Q8" s="6">
-        <v>0</v>
-      </c>
-      <c r="R8" s="14">
-        <v>1.1856300170858387</v>
-      </c>
-      <c r="S8" s="6">
-        <v>1</v>
-      </c>
-      <c r="T8" s="6">
-        <v>1</v>
-      </c>
-      <c r="U8" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="V8" s="6">
-        <v>1.2</v>
-      </c>
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A9" s="12">
-        <v>8</v>
-      </c>
-      <c r="B9" s="6">
-        <v>480</v>
-      </c>
-      <c r="C9" s="5">
-        <v>10</v>
-      </c>
-      <c r="D9" s="5">
-        <v>12</v>
-      </c>
-      <c r="E9" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="F9" s="5">
-        <v>2</v>
-      </c>
-      <c r="G9" s="13">
-        <v>3500</v>
-      </c>
-      <c r="H9" s="11">
-        <v>0</v>
-      </c>
-      <c r="I9" s="6">
-        <v>20</v>
-      </c>
-      <c r="J9" s="6">
-        <v>0</v>
-      </c>
-      <c r="K9" s="14">
-        <v>1.1856300170858387</v>
-      </c>
-      <c r="L9" s="6">
-        <v>1</v>
-      </c>
-      <c r="M9" s="6">
-        <v>1</v>
-      </c>
-      <c r="N9" s="6">
-        <v>0.7</v>
-      </c>
-      <c r="O9" s="6">
-        <v>1.2</v>
-      </c>
-      <c r="P9" s="6">
-        <v>20</v>
-      </c>
-      <c r="Q9" s="6">
-        <v>0</v>
-      </c>
-      <c r="R9" s="14">
-        <v>1.1856300170858387</v>
-      </c>
-      <c r="S9" s="6">
-        <v>1</v>
-      </c>
-      <c r="T9" s="6">
-        <v>1</v>
-      </c>
-      <c r="U9" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="V9" s="6">
-        <v>1.2</v>
-      </c>
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10" s="12">
-        <v>9</v>
-      </c>
-      <c r="B10" s="6">
-        <v>480</v>
-      </c>
-      <c r="C10" s="5">
-        <v>10</v>
-      </c>
-      <c r="D10" s="5">
-        <v>12</v>
-      </c>
-      <c r="E10" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="F10" s="5">
-        <v>2</v>
-      </c>
-      <c r="G10" s="13">
-        <v>3500</v>
-      </c>
-      <c r="H10" s="11">
-        <v>0</v>
-      </c>
-      <c r="I10" s="6">
-        <v>20</v>
-      </c>
-      <c r="J10" s="6">
-        <v>0</v>
-      </c>
-      <c r="K10" s="14">
-        <v>2.4700625355954968</v>
-      </c>
-      <c r="L10" s="6">
-        <v>1</v>
-      </c>
-      <c r="M10" s="6">
-        <v>1</v>
-      </c>
-      <c r="N10" s="6">
-        <v>0.7</v>
-      </c>
-      <c r="O10" s="6">
-        <v>1.2</v>
-      </c>
-      <c r="P10" s="6">
-        <v>20</v>
-      </c>
-      <c r="Q10" s="6">
-        <v>0</v>
-      </c>
-      <c r="R10" s="14">
-        <v>2.4700625355954968</v>
-      </c>
-      <c r="S10" s="6">
-        <v>1</v>
-      </c>
-      <c r="T10" s="6">
-        <v>1</v>
-      </c>
-      <c r="U10" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="V10" s="6">
-        <v>1.2</v>
-      </c>
+    <row r="10" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A11" s="12">
-        <v>10</v>
-      </c>
-      <c r="B11" s="6">
-        <v>208</v>
-      </c>
-      <c r="C11" s="5">
-        <v>10</v>
-      </c>
-      <c r="D11" s="5">
-        <v>12</v>
-      </c>
-      <c r="E11" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="F11" s="5">
-        <v>2</v>
-      </c>
-      <c r="G11" s="13">
-        <v>3500</v>
-      </c>
-      <c r="H11" s="11">
-        <v>0</v>
-      </c>
-      <c r="I11" s="6">
-        <v>20</v>
-      </c>
-      <c r="J11" s="6">
-        <v>0</v>
-      </c>
-      <c r="K11" s="14">
-        <v>2.4700625355954968</v>
-      </c>
-      <c r="L11" s="6">
-        <v>1</v>
-      </c>
-      <c r="M11" s="6">
-        <v>1</v>
-      </c>
-      <c r="N11" s="6">
-        <v>0.7</v>
-      </c>
-      <c r="O11" s="6">
-        <v>1.2</v>
-      </c>
-      <c r="P11" s="6">
-        <v>20</v>
-      </c>
-      <c r="Q11" s="6">
-        <v>0</v>
-      </c>
-      <c r="R11" s="14">
-        <v>2.4700625355954968</v>
-      </c>
-      <c r="S11" s="6">
-        <v>1</v>
-      </c>
-      <c r="T11" s="6">
-        <v>1</v>
-      </c>
-      <c r="U11" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="V11" s="6">
-        <v>1.2</v>
-      </c>
+    <row r="11" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A12" s="12">
-        <v>11</v>
-      </c>
-      <c r="B12" s="6">
-        <v>208</v>
-      </c>
-      <c r="C12" s="5">
-        <v>10</v>
-      </c>
-      <c r="D12" s="5">
-        <v>12</v>
-      </c>
-      <c r="E12" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="F12" s="5">
-        <v>2</v>
-      </c>
-      <c r="G12" s="13">
-        <v>3500</v>
-      </c>
-      <c r="H12" s="11">
-        <v>0</v>
-      </c>
-      <c r="I12" s="6">
-        <v>20</v>
-      </c>
-      <c r="J12" s="6">
-        <v>0</v>
-      </c>
-      <c r="K12" s="14">
-        <v>2.4700625355954968</v>
-      </c>
-      <c r="L12" s="6">
-        <v>1</v>
-      </c>
-      <c r="M12" s="6">
-        <v>1</v>
-      </c>
-      <c r="N12" s="6">
-        <v>0.7</v>
-      </c>
-      <c r="O12" s="6">
-        <v>1.2</v>
-      </c>
-      <c r="P12" s="6">
-        <v>20</v>
-      </c>
-      <c r="Q12" s="6">
-        <v>0</v>
-      </c>
-      <c r="R12" s="14">
-        <v>2.4700625355954968</v>
-      </c>
-      <c r="S12" s="6">
-        <v>1</v>
-      </c>
-      <c r="T12" s="6">
-        <v>1</v>
-      </c>
-      <c r="U12" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="V12" s="6">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A13" s="12">
-        <v>12</v>
-      </c>
-      <c r="B13" s="6">
-        <v>208</v>
-      </c>
-      <c r="C13" s="5">
-        <v>10</v>
-      </c>
-      <c r="D13" s="5">
-        <v>12</v>
-      </c>
-      <c r="E13" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="F13" s="5">
-        <v>2</v>
-      </c>
-      <c r="G13" s="13">
-        <v>3500</v>
-      </c>
-      <c r="H13" s="11">
-        <v>0</v>
-      </c>
-      <c r="I13" s="6">
-        <v>20</v>
-      </c>
-      <c r="J13" s="6">
-        <v>0</v>
-      </c>
-      <c r="K13" s="14">
-        <v>2.4700625355954968</v>
-      </c>
-      <c r="L13" s="6">
-        <v>1</v>
-      </c>
-      <c r="M13" s="6">
-        <v>1</v>
-      </c>
-      <c r="N13" s="6">
-        <v>0.7</v>
-      </c>
-      <c r="O13" s="6">
-        <v>1.2</v>
-      </c>
-      <c r="P13" s="6">
-        <v>20</v>
-      </c>
-      <c r="Q13" s="6">
-        <v>0</v>
-      </c>
-      <c r="R13" s="14">
-        <v>2.4700625355954968</v>
-      </c>
-      <c r="S13" s="6">
-        <v>1</v>
-      </c>
-      <c r="T13" s="6">
-        <v>1</v>
-      </c>
-      <c r="U13" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="V13" s="6">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A14" s="12">
-        <v>13</v>
-      </c>
-      <c r="B14" s="6">
-        <v>208</v>
-      </c>
-      <c r="C14" s="5">
-        <v>10</v>
-      </c>
-      <c r="D14" s="5">
-        <v>12</v>
-      </c>
-      <c r="E14" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="F14" s="5">
-        <v>2</v>
-      </c>
-      <c r="G14" s="13">
-        <v>3500</v>
-      </c>
-      <c r="H14" s="11">
-        <v>0</v>
-      </c>
-      <c r="I14" s="6">
-        <v>20</v>
-      </c>
-      <c r="J14" s="6">
-        <v>0</v>
-      </c>
-      <c r="K14" s="14">
-        <v>2.4700625355954968</v>
-      </c>
-      <c r="L14" s="6">
-        <v>1</v>
-      </c>
-      <c r="M14" s="6">
-        <v>1</v>
-      </c>
-      <c r="N14" s="6">
-        <v>0.7</v>
-      </c>
-      <c r="O14" s="6">
-        <v>1.2</v>
-      </c>
-      <c r="P14" s="6">
-        <v>20</v>
-      </c>
-      <c r="Q14" s="6">
-        <v>0</v>
-      </c>
-      <c r="R14" s="14">
-        <v>2.4700625355954968</v>
-      </c>
-      <c r="S14" s="6">
-        <v>1</v>
-      </c>
-      <c r="T14" s="6">
-        <v>1</v>
-      </c>
-      <c r="U14" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="V14" s="6">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-    </row>
-    <row r="16" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-    </row>
-    <row r="17" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-    </row>
-    <row r="18" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-    </row>
-    <row r="19" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
+    <row r="12" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Created goose lib with publishers and subscribes Updated RemoteCHIL.mdl to use common publisher Repaired F4 relay settings to 208V
</commit_message>
<xml_diff>
--- a/DistributionSystems/SimulinkOpal/Banshee/relay_settings/F4_relay_nrel.xlsx
+++ b/DistributionSystems/SimulinkOpal/Banshee/relay_settings/F4_relay_nrel.xlsx
@@ -1145,7 +1145,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="6">
-        <v>480</v>
+        <v>208</v>
       </c>
       <c r="C6" s="5">
         <v>10</v>
@@ -1213,7 +1213,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="6">
-        <v>480</v>
+        <v>208</v>
       </c>
       <c r="C7" s="5">
         <v>10</v>

</xml_diff>